<commit_message>
Formatting and removal of excess files.
</commit_message>
<xml_diff>
--- a/table/Model 1.xlsx
+++ b/table/Model 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\C++\Science Fair 2025\tests\data\github\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173A0C0C-AC4B-4A4B-9D05-D7255692D512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E9C1EC-3BD7-4700-988A-D840607DE4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3463,13 +3463,14 @@
   <dimension ref="A1:O1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="15" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>